<commit_message>
Updated the contents of various docs
</commit_message>
<xml_diff>
--- a/Sources.xlsx
+++ b/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Capstone 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A0E4124A-4586-402E-B7AF-32CB5DE74B62}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{531F992A-5525-487D-9AD3-750D037FA872}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{83B6082E-9E44-41D9-BB0A-A25EEDCBCFB4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>LIST OF SOURCES FOR THE CAPSTONE PROJECT DOCUMENTATION</t>
   </si>
@@ -73,6 +73,24 @@
   </si>
   <si>
     <t>Link retrieved</t>
+  </si>
+  <si>
+    <t>Chapter 1 - Introduction</t>
+  </si>
+  <si>
+    <t>Link not yet retrieved</t>
+  </si>
+  <si>
+    <t>Hedges</t>
+  </si>
+  <si>
+    <t>Chapter 1 - Description</t>
+  </si>
+  <si>
+    <t>Chapter 1 -Introduction</t>
+  </si>
+  <si>
+    <t>Estonia Election Online</t>
   </si>
 </sst>
 </file>
@@ -183,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,31 +212,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -538,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92398D7-C530-400B-B3F6-7F69DDE151A5}">
   <dimension ref="C4:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10:Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,326 +570,377 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
       <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="10">
         <v>43291</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="11" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="12" t="s">
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="10">
         <v>43291</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="11" t="s">
+      <c r="G8" s="4"/>
+      <c r="H8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="12" t="s">
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="10">
         <v>43299</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="4"/>
+      <c r="H9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3" t="s">
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="C10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="10">
+        <v>43291</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="M16:Q16"/>
-    <mergeCell ref="M17:Q17"/>
-    <mergeCell ref="M18:Q18"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="C4:Q5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H12:L12"/>
     <mergeCell ref="M19:Q19"/>
     <mergeCell ref="H19:L19"/>
     <mergeCell ref="M6:Q6"/>
@@ -885,49 +957,19 @@
     <mergeCell ref="H16:L16"/>
     <mergeCell ref="H17:L17"/>
     <mergeCell ref="H18:L18"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="C4:Q5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="M17:Q17"/>
+    <mergeCell ref="M18:Q18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1" xr:uid="{5F529AA9-04C6-4CFB-992F-811598F7BCCB}"/>
     <hyperlink ref="H8" r:id="rId2" xr:uid="{0DA5ECA3-C672-4B56-A954-AC77135F9636}"/>
     <hyperlink ref="H9" r:id="rId3" xr:uid="{4AB97847-3DE9-482D-81EB-0FE46FF9E347}"/>
+    <hyperlink ref="H11" r:id="rId4" xr:uid="{8E7C0613-0875-47C0-9535-AF413E53F320}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edited chapter 2 and 3
</commit_message>
<xml_diff>
--- a/Sources.xlsx
+++ b/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Capstone 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{531F992A-5525-487D-9AD3-750D037FA872}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{45B9BAAE-1651-4497-8EFE-340D6B100951}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{83B6082E-9E44-41D9-BB0A-A25EEDCBCFB4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>LIST OF SOURCES FOR THE CAPSTONE PROJECT DOCUMENTATION</t>
   </si>
@@ -91,6 +91,66 @@
   </si>
   <si>
     <t>Estonia Election Online</t>
+  </si>
+  <si>
+    <t>Centralized Electronic Voting System</t>
+  </si>
+  <si>
+    <t>Chapter 2 - Foreign Literature</t>
+  </si>
+  <si>
+    <t>International Journal of Computer Applications (0975 – 8887) Volume 179 – No.27, March 2018</t>
+  </si>
+  <si>
+    <t>Online Voting Isn’t as Flawed as You Think—Just Ask Estonia</t>
+  </si>
+  <si>
+    <t>https://spectrum.ieee.org/telecom/internet/online-voting-isnt-as-flawed-as-you-thinkjust-ask-estonia</t>
+  </si>
+  <si>
+    <t>How to Break Web Software: Functional and Security Testing of Web Applications and Web Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike Andrews &amp; James A. Whittaker </t>
+  </si>
+  <si>
+    <t>http://iskwiki.upd.edu.ph/index.php/Online/Automated_Elections_in_the_Philippines#.W2M7bygzbIU</t>
+  </si>
+  <si>
+    <t>Online/Automated Elections in the Philippines</t>
+  </si>
+  <si>
+    <t>https://www.philstar.com/headlines/2010/05/13/574450/automation-critics-happy-be-wrong</t>
+  </si>
+  <si>
+    <t>Automation Critics Happy to be Wrong</t>
+  </si>
+  <si>
+    <t>Chapter 2 - Local Literature - Punay</t>
+  </si>
+  <si>
+    <t>Chapter 2 - Local Literature - Salma Angkaya</t>
+  </si>
+  <si>
+    <t>Tanmay Kadam 2016</t>
+  </si>
+  <si>
+    <t>http://cebudailynews.inquirer.net/41007/filipino-youths-are-biggest-internet-users</t>
+  </si>
+  <si>
+    <t>Chapter 2 - Local Literature</t>
+  </si>
+  <si>
+    <t>Filipino youths are biggest Internet users</t>
+  </si>
+  <si>
+    <t>Chapter 2 - Foreign Studies</t>
+  </si>
+  <si>
+    <t>Estonia Election System - iVoting -Cybernetica</t>
+  </si>
+  <si>
+    <t>Monira Monir Haroon Khater</t>
   </si>
 </sst>
 </file>
@@ -201,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -215,22 +275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -239,7 +284,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -557,365 +650,768 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92398D7-C530-400B-B3F6-7F69DDE151A5}">
-  <dimension ref="C4:Q19"/>
+  <dimension ref="C4:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="40.140625" customWidth="1"/>
     <col min="4" max="5" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="5" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="5" t="s">
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="7"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="10">
+      <c r="E7" s="5"/>
+      <c r="F7" s="12">
         <v>43291</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="9" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="8" t="s">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="10">
+      <c r="E8" s="5"/>
+      <c r="F8" s="12">
         <v>43291</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="9" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="8" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="10">
+      <c r="E9" s="5"/>
+      <c r="F9" s="12">
         <v>43299</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4" t="s">
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="10">
+      <c r="E11" s="5"/>
+      <c r="F11" s="12">
         <v>43291</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="9" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
+      <c r="C14" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="12">
+        <v>43313</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="12">
+        <v>43313</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
+      <c r="C16" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="12">
+        <v>43313</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="12">
+        <v>43313</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="12">
+        <v>43313</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C19" s="2"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="12">
+        <v>43313</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="17"/>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="12">
+        <v>43313</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="12">
+        <v>43313</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="17"/>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="17"/>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="17"/>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="17"/>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C25" s="4"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="17"/>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="17"/>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="17"/>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="17"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C29" s="4"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="17"/>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="17"/>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="4"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="17"/>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="17"/>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="17"/>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="C4:Q5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
+  <mergeCells count="117">
+    <mergeCell ref="M31:Q31"/>
+    <mergeCell ref="M32:Q32"/>
+    <mergeCell ref="M33:Q33"/>
+    <mergeCell ref="M26:Q26"/>
+    <mergeCell ref="M27:Q27"/>
+    <mergeCell ref="M28:Q28"/>
+    <mergeCell ref="M29:Q29"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="M21:Q21"/>
+    <mergeCell ref="M22:Q22"/>
+    <mergeCell ref="M23:Q23"/>
+    <mergeCell ref="M24:Q24"/>
+    <mergeCell ref="M25:Q25"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H24:L24"/>
+    <mergeCell ref="H25:L25"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="M34:Q34"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:L34"/>
     <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="M17:Q17"/>
+    <mergeCell ref="M18:Q18"/>
+    <mergeCell ref="M20:Q20"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="M9:Q9"/>
+    <mergeCell ref="M10:Q10"/>
+    <mergeCell ref="M11:Q11"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="D20:E20"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
@@ -931,45 +1427,29 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="M9:Q9"/>
-    <mergeCell ref="M10:Q10"/>
-    <mergeCell ref="M11:Q11"/>
-    <mergeCell ref="M12:Q12"/>
-    <mergeCell ref="M13:Q13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="M16:Q16"/>
-    <mergeCell ref="M17:Q17"/>
-    <mergeCell ref="M18:Q18"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="C4:Q5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1" xr:uid="{5F529AA9-04C6-4CFB-992F-811598F7BCCB}"/>
     <hyperlink ref="H8" r:id="rId2" xr:uid="{0DA5ECA3-C672-4B56-A954-AC77135F9636}"/>
     <hyperlink ref="H9" r:id="rId3" xr:uid="{4AB97847-3DE9-482D-81EB-0FE46FF9E347}"/>
     <hyperlink ref="H11" r:id="rId4" xr:uid="{8E7C0613-0875-47C0-9535-AF413E53F320}"/>
+    <hyperlink ref="H14" r:id="rId5" xr:uid="{997B5058-2E06-432C-9BB2-BAE9D202A21D}"/>
+    <hyperlink ref="H16" r:id="rId6" location=".W2M7bygzbIU" xr:uid="{3F3F2C56-7F1B-4FBA-9B59-159E64D67251}"/>
+    <hyperlink ref="C16" r:id="rId7" display="http://iskwiki.upd.edu.ph/index.php/Online/Automated_Elections_in_the_Philippines" xr:uid="{15CA7A75-F9A5-4096-82CC-E595E67E8910}"/>
+    <hyperlink ref="H17" r:id="rId8" xr:uid="{D42D3A92-FC54-4CD4-A44C-9E372BBA7205}"/>
+    <hyperlink ref="H19" r:id="rId9" xr:uid="{BEFF0F08-F9A3-46B5-9E7A-95D198C3F092}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>